<commit_message>
find max inverst potential
</commit_message>
<xml_diff>
--- a/Ефанов Михаил Александрович/Курсовая работа/Предложения.xlsx
+++ b/Ефанов Михаил Александрович/Курсовая работа/Предложения.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89AE2B84-AD20-424A-8713-9ECE81C35BD8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{693C6B65-FDFF-426B-A03B-AE87A9F777B2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -358,7 +358,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>